<commit_message>
added BOS passenger type
</commit_message>
<xml_diff>
--- a/backend/bak/e-Ticket Issue Form Data Record (251128).xlsx
+++ b/backend/bak/e-Ticket Issue Form Data Record (251128).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\airline-ticket-printing-system\backend\bak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51680178-7136-4888-BCD6-166EE2ED6810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4FE3E2-9AEB-4220-A943-A945EFFA7FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="705" windowWidth="21600" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CHD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>INF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -176,6 +172,9 @@
   </si>
   <si>
     <t>01DEC2025</t>
+  </si>
+  <si>
+    <t>BOS</t>
   </si>
 </sst>
 </file>
@@ -585,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -611,16 +610,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>6</v>
@@ -629,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>8</v>
@@ -638,7 +637,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>8</v>
@@ -647,22 +646,22 @@
         <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="R1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -673,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -685,25 +684,25 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="4"/>
@@ -718,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -730,43 +729,43 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
         <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -777,55 +776,55 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" t="s">
         <v>19</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>20</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -836,55 +835,55 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>20</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -898,52 +897,52 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
         <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:19">

</xml_diff>